<commit_message>
Added Fixes necessary for TVG
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/Inventory Item Template_MFG FINAL.xlsx
+++ b/src/main/resources/templates/Inventory Item Template_MFG FINAL.xlsx
@@ -8,20 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\Documents\DataProcessing\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35B7042-F493-472A-933D-AE3EF0E0B7B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1650DD6-2F61-42CD-AD4D-B9AA232A0139}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Field Restrictions" sheetId="2" r:id="rId1"/>
     <sheet name="Serialized &amp; Lot Numbered  Inve" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="395">
   <si>
     <t>Bill Quantity Variance Account</t>
   </si>
@@ -3056,6 +3066,36 @@
   </si>
   <si>
     <t>Max 99 chars</t>
+  </si>
+  <si>
+    <t>replacementCost</t>
+  </si>
+  <si>
+    <t>Replacement Cost</t>
+  </si>
+  <si>
+    <t>cogsaccount_name</t>
+  </si>
+  <si>
+    <t>incomeaccount_name</t>
+  </si>
+  <si>
+    <t>assetaccount_name</t>
+  </si>
+  <si>
+    <t>billpricevarianceacct_name</t>
+  </si>
+  <si>
+    <t>billqtyvarianceacct_name</t>
+  </si>
+  <si>
+    <t>billexchratevarianceacct_name</t>
+  </si>
+  <si>
+    <t>custreturnvarianceaccount_name</t>
+  </si>
+  <si>
+    <t>vendreturnvarianceaccount_name</t>
   </si>
 </sst>
 </file>
@@ -4389,10 +4429,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:DF10"/>
+  <dimension ref="A1:DO10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CZ1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:DF1"/>
+    <sheetView tabSelected="1" topLeftCell="DI1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="DN8" sqref="DN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4456,21 +4496,21 @@
     <col min="93" max="93" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="27.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="35.42578125" style="17" customWidth="1"/>
-    <col min="97" max="97" width="41.42578125" style="1" customWidth="1"/>
-    <col min="98" max="98" width="38.7109375" style="1" customWidth="1"/>
-    <col min="99" max="99" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="36" style="1" customWidth="1"/>
-    <col min="101" max="101" width="35.5703125" style="1" customWidth="1"/>
-    <col min="102" max="102" width="30.7109375" style="1"/>
-    <col min="103" max="105" width="36.85546875" style="1" customWidth="1"/>
-    <col min="106" max="106" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="28.85546875" style="1" customWidth="1"/>
-    <col min="108" max="110" width="45" style="1" bestFit="1" customWidth="1"/>
-    <col min="111" max="16384" width="30.7109375" style="1"/>
+    <col min="96" max="97" width="35.42578125" style="17" customWidth="1"/>
+    <col min="98" max="99" width="41.42578125" style="1" customWidth="1"/>
+    <col min="100" max="101" width="38.7109375" style="1" customWidth="1"/>
+    <col min="102" max="102" width="36" style="1" bestFit="1" customWidth="1"/>
+    <col min="103" max="105" width="36" style="1" customWidth="1"/>
+    <col min="106" max="107" width="35.5703125" style="1" customWidth="1"/>
+    <col min="108" max="109" width="30.7109375" style="1"/>
+    <col min="110" max="113" width="36.85546875" style="1" customWidth="1"/>
+    <col min="114" max="114" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="28.85546875" style="1" customWidth="1"/>
+    <col min="116" max="118" width="45" style="1" bestFit="1" customWidth="1"/>
+    <col min="119" max="16384" width="30.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:110" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:119" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>278</v>
       </c>
@@ -4759,50 +4799,77 @@
       <c r="CR1" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="CS1" s="6" t="s">
+      <c r="CS1" s="22" t="s">
         <v>351</v>
       </c>
       <c r="CT1" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="CU1" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="CU1" s="6" t="s">
+      <c r="CV1" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="CW1" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="CV1" s="3" t="s">
+      <c r="CX1" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="CY1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="CW1" s="3" t="s">
+      <c r="CZ1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="DA1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="CX1" s="3" t="s">
+      <c r="DB1" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="DC1" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="DD1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="CY1" s="3" t="s">
+      <c r="DE1" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="CZ1" s="3" t="s">
+      <c r="DF1" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="DG1" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="DA1" s="3" t="s">
+      <c r="DH1" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="DI1" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="DB1" s="13" t="s">
+      <c r="DJ1" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="DC1" s="6" t="s">
+      <c r="DK1" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="DD1" s="6" t="s">
+      <c r="DL1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="DE1" s="6" t="s">
+      <c r="DM1" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="DF1" s="6" t="s">
+      <c r="DN1" s="6" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="2" spans="1:110" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="DO1" s="6" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:119" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>108</v>
       </c>
@@ -5091,50 +5158,54 @@
       <c r="CR2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="CS2" s="6" t="s">
+      <c r="CS2" s="13"/>
+      <c r="CT2" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="CT2" s="6" t="s">
+      <c r="CV2" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="CU2" s="6" t="s">
+      <c r="CX2" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="CV2" s="6" t="s">
+      <c r="CZ2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="CW2" s="6" t="s">
+      <c r="DB2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="CX2" s="6" t="s">
+      <c r="DD2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="CY2" s="6" t="s">
+      <c r="DF2" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="CZ2" s="6" t="s">
+      <c r="DH2" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="DA2" s="6" t="s">
+      <c r="DI2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="DB2" s="13" t="s">
+      <c r="DJ2" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="DC2" s="6" t="s">
+      <c r="DK2" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="DD2" s="6" t="s">
+      <c r="DL2" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="DE2" s="6" t="s">
+      <c r="DM2" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="DF2" s="6" t="s">
+      <c r="DN2" s="6" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="3" spans="1:110" s="19" customFormat="1" ht="289.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="DO2" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="3" spans="1:119" s="19" customFormat="1" ht="289.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
         <v>363</v>
       </c>
@@ -5423,50 +5494,61 @@
       <c r="CR3" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="CS3" s="20" t="s">
+      <c r="CS3" s="20"/>
+      <c r="CT3" s="20" t="s">
         <v>234</v>
       </c>
-      <c r="CT3" s="20" t="s">
+      <c r="CU3" s="20"/>
+      <c r="CV3" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="CU3" s="20" t="s">
+      <c r="CW3" s="20"/>
+      <c r="CX3" s="20" t="s">
         <v>236</v>
       </c>
-      <c r="CV3" s="20" t="s">
+      <c r="CY3" s="20"/>
+      <c r="CZ3" s="20" t="s">
         <v>237</v>
       </c>
-      <c r="CW3" s="20" t="s">
+      <c r="DA3" s="20"/>
+      <c r="DB3" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="CX3" s="20" t="s">
+      <c r="DC3" s="20"/>
+      <c r="DD3" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="CY3" s="20" t="s">
+      <c r="DE3" s="20"/>
+      <c r="DF3" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="CZ3" s="20" t="s">
+      <c r="DG3" s="20"/>
+      <c r="DH3" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="DA3" s="20" t="s">
+      <c r="DI3" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="DB3" s="20" t="s">
+      <c r="DJ3" s="20" t="s">
         <v>264</v>
       </c>
-      <c r="DC3" s="20" t="s">
+      <c r="DK3" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="DD3" s="20" t="s">
+      <c r="DL3" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="DE3" s="20" t="s">
+      <c r="DM3" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="DF3" s="20" t="s">
+      <c r="DN3" s="20" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="4" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DO3" s="20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>103</v>
       </c>
@@ -5740,50 +5822,54 @@
       <c r="CR4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="CS4" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="CS4" s="1"/>
       <c r="CT4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CU4" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="CV4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CW4" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="CX4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CY4" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="CZ4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DA4" s="1" t="s">
+      <c r="DB4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DD4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DF4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DH4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DI4" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DB4" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="DC4" s="1" t="s">
+      <c r="DJ4" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="DK4" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="DD4" s="1" t="s">
+      <c r="DL4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DE4" s="1" t="s">
+      <c r="DM4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DF4" s="1" t="s">
+      <c r="DN4" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:110" x14ac:dyDescent="0.2">
+      <c r="DO4" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>109</v>
       </c>
@@ -5979,44 +6065,44 @@
       <c r="CP5" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CS5" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="CT5" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CU5" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="CV5" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CW5" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="CX5" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CY5" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="CZ5" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DA5" s="1" t="s">
+      <c r="DB5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DD5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DF5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DH5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="DI5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DB5" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="DC5" s="1" t="s">
+      <c r="DJ5" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="DK5" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DF5" s="1" t="s">
+      <c r="DN5" s="1" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="6" spans="1:110" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:119" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>126</v>
       </c>
@@ -6042,20 +6128,21 @@
       <c r="CJ6" s="35"/>
       <c r="CN6" s="35"/>
       <c r="CR6" s="35"/>
-      <c r="CS6" s="14" t="s">
+      <c r="CS6" s="35"/>
+      <c r="CT6" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="CT6" s="14" t="s">
+      <c r="CV6" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="CU6" s="14" t="s">
+      <c r="CX6" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="DB6" s="5" t="s">
+      <c r="DJ6" s="5" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="7" spans="1:110" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:119" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>125</v>
       </c>
@@ -6083,20 +6170,21 @@
       <c r="CJ7" s="35"/>
       <c r="CN7" s="35"/>
       <c r="CR7" s="35"/>
-      <c r="CS7" s="14" t="s">
+      <c r="CS7" s="35"/>
+      <c r="CT7" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="CT7" s="14" t="s">
+      <c r="CV7" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="CU7" s="14" t="s">
+      <c r="CX7" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="DB7" s="5" t="s">
+      <c r="DJ7" s="5" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="8" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>134</v>
       </c>
@@ -6121,11 +6209,11 @@
       <c r="AQ8" s="33"/>
       <c r="AR8" s="33"/>
       <c r="AS8" s="33"/>
-      <c r="DA8" s="1" t="s">
+      <c r="DI8" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="9" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>117</v>
       </c>
@@ -6139,7 +6227,7 @@
       <c r="AR9" s="32"/>
       <c r="AS9" s="32"/>
     </row>
-    <row r="10" spans="1:110" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:119" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>119</v>
       </c>

</xml_diff>